<commit_message>
Oct 29, 2024, 8:10 AM
</commit_message>
<xml_diff>
--- a/Hải Trần's folder/extract + save data/hako_dataset.xlsx
+++ b/Hải Trần's folder/extract + save data/hako_dataset.xlsx
@@ -613,37 +613,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Đọc Seirei Tsukai no Blade Dance - Chương 1: Ngươi là tinh linh của ta! - Cổng Light Novel</t>
+          <t>Seirei Tsukai no Blade Dance</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://ln.hako.re/truyen/1-seirei-tsukai-no-blade-dance/c1-chuong-1-nguoi-la-tinh-linh-cua-ta</t>
+          <t>https://ln.hako.vn/truyen/1-seirei-tsukai-no-blade-dance</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Truyện dịch</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Action', 'Adventure', 'Comedy', 'Fantasy', 'Romance', 'Ecchi', 'Harem', 'School Life', 'Super Power', '']</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Not sure</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Not sure</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Not sure</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -658,12 +658,12 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Shimizu Yuu</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Sakura Hanpen, Nimura Yuuji, Shimesada Kohada</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -673,14 +673,14 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Đã hoàn thành</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>2944</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>1071757</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
@@ -694,12 +694,12 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>medassin</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/thanh-vien/39</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -709,12 +709,12 @@
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Sonata no Koe</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/nhom-dich/3-sonata-no-koe</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
@@ -733,40 +733,28 @@
         </is>
       </c>
       <c r="AA2" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AB2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
+        <v>272</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>11</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>2016</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>7</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>2020</v>
       </c>
     </row>
     <row r="3">
@@ -777,22 +765,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Đọc Seirei Tsukai no Blade Dance - Phần kết - Cổng Light Novel</t>
+          <t>Utsuro no Hako to Zero no Maria</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://ln.hako.re/truyen/1-seirei-tsukai-no-blade-dance/c10-phan-ket</t>
+          <t>https://ln.hako.vn/truyen/10-utsuro-no-hako-to-zero-no-maria</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Truyện dịch</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Drama', 'Mystery', 'Romance']</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -822,12 +810,12 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Mikage Eiji</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Tetsuo (415)</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -837,18 +825,18 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Tạm ngưng</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>889</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>333710</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Hakomari</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -858,12 +846,12 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>EmbersGlow</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/thanh-vien/1</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -873,12 +861,12 @@
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Solarius</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/nhom-dich/8-solarius</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
@@ -897,40 +885,28 @@
         </is>
       </c>
       <c r="AA3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AB3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
+        <v>25</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>11</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>2016</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>11</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>2016</v>
       </c>
     </row>
     <row r="4">
@@ -941,22 +917,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Đọc Seirei Tsukai no Blade Dance - Chương 5 - Vũ khí Tinh Linh - Cổng Light Novel</t>
+          <t>Accel World</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://ln.hako.re/truyen/1-seirei-tsukai-no-blade-dance/c100-chuong-5-vu-khi-tinh-linh</t>
+          <t>https://ln.hako.vn/truyen/100-accel-world</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Truyện dịch</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Action', 'Harem', 'School Life', 'Science Fiction', 'Romance']</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -986,12 +962,12 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Reki Kawahara</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>HIMA</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -1001,14 +977,14 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Tạm ngưng</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>90591</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
@@ -1022,12 +998,12 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>EmbersGlow</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/thanh-vien/1</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -1037,12 +1013,12 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Sonata no Koe</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/nhom-dich/3-sonata-no-koe</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
@@ -1061,40 +1037,28 @@
         </is>
       </c>
       <c r="AA4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
+        <v>14</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>2016</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>2016</v>
       </c>
     </row>
     <row r="5">
@@ -1105,22 +1069,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Đọc Seirei Tsukai no Blade Dance - Chương 6 - Scarlet Valkyrie - Cổng Light Novel</t>
+          <t>Psycho Love Comedy</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://ln.hako.re/truyen/1-seirei-tsukai-no-blade-dance/c101-chuong-6-scarlet-valkyrie</t>
+          <t>https://ln.hako.vn/truyen/101-psycho-love-comedy</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Truyện dịch</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Comedy', 'Harem', 'School Life', 'Romance']</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1150,12 +1114,12 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Mizuki Mizushiro</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Namanie</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -1165,18 +1129,18 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Đang tiến hành</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>237</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>47955</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Psycome</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -1186,12 +1150,12 @@
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>EmbersGlow</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/thanh-vien/1</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
@@ -1201,12 +1165,12 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Sonata no Koe</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/nhom-dich/3-sonata-no-koe</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
@@ -1225,40 +1189,28 @@
         </is>
       </c>
       <c r="AA5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AH5" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>11</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>2016</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>14</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>11</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>2016</v>
       </c>
     </row>
     <row r="6">
@@ -1269,22 +1221,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Đọc Seirei Tsukai no Blade Dance - Chương 7 - Cross Fire - Cổng Light Novel</t>
+          <t>A Simple Survey</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://ln.hako.re/truyen/1-seirei-tsukai-no-blade-dance/c102-chuong-7-cross-fire</t>
+          <t>https://ln.hako.vn/truyen/102-a-simple-survey</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Truyện dịch</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Horror', 'Mystery', 'Supernatural', 'Fantasy', 'Science Fiction', 'Suspense']</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1314,12 +1266,12 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Kamachi Kazuma</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Haimura Kiyotaka</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -1329,14 +1281,14 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Đã hoàn thành</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>82382</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
@@ -1350,12 +1302,12 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>EmbersGlow</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/thanh-vien/1</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -1365,12 +1317,12 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Sonata no Koe</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/nhom-dich/3-sonata-no-koe</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
@@ -1389,40 +1341,28 @@
         </is>
       </c>
       <c r="AA6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AD6" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AE6" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AF6" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AG6" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AH6" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
+        <v>34</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>11</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>2016</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>11</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>2016</v>
       </c>
     </row>
     <row r="7">
@@ -1433,22 +1373,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Đọc Seirei Tsukai no Blade Dance - Kết - Cổng Light Novel</t>
+          <t>Clockwork Planet</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://ln.hako.re/truyen/1-seirei-tsukai-no-blade-dance/c103-ket</t>
+          <t>https://ln.hako.vn/truyen/103-clockwork-planet</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Truyện dịch</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Drama', 'Fantasy', 'Science Fiction', 'Romance']</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1478,12 +1418,12 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Tsubaki Himana</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Shino</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -1493,18 +1433,18 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Đang tiến hành</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>167</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>40130</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>クロックワーク・プラネット</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1514,12 +1454,12 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>EmbersGlow</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/thanh-vien/1</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
@@ -1529,12 +1469,12 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Sonata no Koe</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/nhom-dich/3-sonata-no-koe</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
@@ -1553,40 +1493,28 @@
         </is>
       </c>
       <c r="AA7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AD7" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AE7" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AF7" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AG7" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AH7" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
+        <v>5</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>11</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>2016</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>2017</v>
       </c>
     </row>
     <row r="8">
@@ -1597,22 +1525,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Đọc Seirei Tsukai no Blade Dance - Lời bạt - Cổng Light Novel</t>
+          <t>All you need is kill</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://ln.hako.re/truyen/1-seirei-tsukai-no-blade-dance/c104-chuong-10</t>
+          <t>https://ln.hako.vn/truyen/104-all-you-need-is-kill</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Truyện dịch</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Science Fiction', 'Action', 'Mecha', 'Mystery', 'Tragedy', 'Romance', 'Psychological', '']</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1642,12 +1570,12 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Hiroshi Sakurazaka</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Takeshi Obata, Yoshitoshi ABe</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1657,18 +1585,18 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Đã hoàn thành</t>
         </is>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>75053</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Chỉ việc giết là được</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1678,12 +1606,12 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>EmbersGlow</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/thanh-vien/1</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -1693,12 +1621,12 @@
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Sonata no Koe</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/nhom-dich/3-sonata-no-koe</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
@@ -1717,40 +1645,28 @@
         </is>
       </c>
       <c r="AA8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC8" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AD8" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AE8" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AF8" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AG8" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AH8" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
+        <v>5</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>11</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>2016</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>11</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>2016</v>
       </c>
     </row>
     <row r="9">
@@ -1761,22 +1677,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Đọc Seirei Tsukai no Blade Dance - Mở đầu - Cổng Light Novel</t>
+          <t>Yahari Ore no Seishun Love Come wa Machigatteiru</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://ln.hako.re/truyen/1-seirei-tsukai-no-blade-dance/c105-mo-dau</t>
+          <t>https://ln.hako.vn/truyen/108-yahari-ore-no-seishun-love-come-wa-machigatteiru</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Truyện dịch</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Comedy', 'Drama', 'School Life', 'Slice of Life', 'Romance']</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1806,12 +1722,12 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Wataru Watari</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Ponkan⑧</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1821,18 +1737,18 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Đang tiến hành</t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>540</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>348338</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>OreGairu</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1842,12 +1758,12 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>EmbersGlow</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/thanh-vien/1</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
@@ -1857,12 +1773,12 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Sonata no Koe</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/nhom-dich/3-sonata-no-koe</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
@@ -1881,40 +1797,28 @@
         </is>
       </c>
       <c r="AA9" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AB9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC9" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AD9" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AE9" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AF9" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AG9" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AH9" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
+        <v>41</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>2016</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>27</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>2016</v>
       </c>
     </row>
     <row r="10">
@@ -1925,22 +1829,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Đọc Seirei Tsukai no Blade Dance - Chương 1 - Muir Alenstarl - Cổng Light Novel</t>
+          <t>Fate/Zero</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://ln.hako.re/truyen/1-seirei-tsukai-no-blade-dance/c106-chuong-1-muir-alenstarl</t>
+          <t>https://ln.hako.vn/truyen/11-fatezero</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Truyện dịch</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Action', 'Fantasy', 'Supernatural', 'Drama']</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1970,12 +1874,12 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Gen Urobuchi</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Takeuchi Takashi</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1985,14 +1889,14 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Đã hoàn thành</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>190</v>
       </c>
       <c r="P10" t="n">
-        <v>0</v>
+        <v>366178</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
@@ -2006,12 +1910,12 @@
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Hako-chan</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/thanh-vien/2</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -2021,12 +1925,12 @@
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Vnsharing</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/nhom-dich/9-vnsharing</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
@@ -2045,40 +1949,28 @@
         </is>
       </c>
       <c r="AA10" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AB10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC10" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AD10" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AE10" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AF10" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AG10" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AH10" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
+        <v>27</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>11</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>2016</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>8</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>2017</v>
       </c>
     </row>
     <row r="11">
@@ -2089,22 +1981,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Đọc Seirei Tsukai no Blade Dance - Chương 2 - Tiếng gọi của Bóng Tối - Cổng Light Novel</t>
+          <t>Chuunibyou Demo Koi ga Shitai!</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://ln.hako.re/truyen/1-seirei-tsukai-no-blade-dance/c107-chuong-2-tieng-goi-cua-bong-toi</t>
+          <t>https://ln.hako.vn/truyen/110-chuunibyou-demo-koi-ga-shitai</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Truyện dịch</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Comedy', 'School Life', 'Romance']</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -2134,12 +2026,12 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Torako</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Nozomi Ousaka</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -2149,18 +2041,18 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Đang tiến hành</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>208476</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Cuồng dâm sinh hoang tưởng vẫn muốn hưởng tình yêu</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -2170,12 +2062,12 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>EmbersGlow</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/thanh-vien/1</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
@@ -2185,64 +2077,52 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Sonata no Koe</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/nhom-dich/3-sonata-no-koe</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>None</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>Zennomi</t>
         </is>
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>https://ln.hako.vn/thanh-vien/3855</t>
         </is>
       </c>
       <c r="AA11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC11" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AD11" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AE11" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AF11" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AG11" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-      <c r="AH11" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
+        <v>36</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>11</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>2016</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>26</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>12</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>2018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>